<commit_message>
mobile user_attation bug fix
</commit_message>
<xml_diff>
--- a/res/east20160309.xlsx
+++ b/res/east20160309.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5306" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5306" uniqueCount="2625">
   <si>
     <t/>
   </si>
@@ -7511,10 +7511,6 @@
   </si>
   <si>
     <t>统,大皮,小皮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根,公斤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -8415,6 +8411,14 @@
   </si>
   <si>
     <t>条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公斤,克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条,公斤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8842,8 +8846,8 @@
   <dimension ref="A1:G994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A845" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G274" sqref="G274"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G260" sqref="G260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -8939,7 +8943,7 @@
         <v>2422</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
@@ -8962,7 +8966,7 @@
         <v>2423</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
@@ -9205,7 +9209,7 @@
         <v>2431</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="7" t="s">
@@ -9289,7 +9293,7 @@
         <v>2431</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>72</v>
@@ -9417,7 +9421,7 @@
         <v>2416</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="7" t="s">
@@ -9610,7 +9614,7 @@
         <v>2439</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>116</v>
@@ -9719,7 +9723,7 @@
         <v>2442</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="7" t="s">
@@ -10001,10 +10005,10 @@
         <v>175</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>2526</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>2527</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>2528</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>176</v>
@@ -10115,7 +10119,7 @@
         <v>2448</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>190</v>
@@ -10161,7 +10165,7 @@
         <v>2450</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>197</v>
@@ -10228,7 +10232,7 @@
         <v>2452</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="7" t="s">
@@ -10538,7 +10542,7 @@
         <v>256</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="7" t="s">
@@ -10647,7 +10651,7 @@
         <v>275</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>276</v>
@@ -10865,7 +10869,7 @@
         <v>315</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="7" t="s">
@@ -10907,7 +10911,7 @@
         <v>322</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="7" t="s">
@@ -10928,7 +10932,7 @@
         <v>2459</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="7" t="s">
@@ -11382,7 +11386,7 @@
         <v>400</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>401</v>
@@ -11498,7 +11502,7 @@
         <v>2409</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="7" t="s">
@@ -11630,7 +11634,7 @@
         <v>444</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="F127" s="2"/>
       <c r="G127" s="7" t="s">
@@ -12469,7 +12473,7 @@
         <v>581</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>582</v>
@@ -12534,7 +12538,7 @@
         <v>2470</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>589</v>
@@ -14450,7 +14454,7 @@
       </c>
       <c r="F259" s="2"/>
       <c r="G259" s="7" t="s">
-        <v>2476</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.15">
@@ -14490,7 +14494,7 @@
       </c>
       <c r="F261" s="2"/>
       <c r="G261" s="7" t="s">
-        <v>839</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.15">
@@ -14624,7 +14628,7 @@
         <v>859</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
@@ -14912,7 +14916,7 @@
         <v>890</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="E282" s="2" t="s">
         <v>33</v>
@@ -15125,7 +15129,7 @@
       <c r="E292" s="2"/>
       <c r="F292" s="2"/>
       <c r="G292" s="7" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.15">
@@ -15139,7 +15143,7 @@
         <v>918</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="E293" s="2"/>
       <c r="F293" s="2"/>
@@ -17253,7 +17257,7 @@
         <v>1167</v>
       </c>
       <c r="E394" s="2" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="F394" s="2" t="s">
         <v>1168</v>
@@ -17273,7 +17277,7 @@
         <v>1170</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="E395" s="2" t="s">
         <v>158</v>
@@ -17355,7 +17359,7 @@
         <v>1178</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="E399" s="2"/>
       <c r="F399" s="2" t="s">
@@ -17843,7 +17847,7 @@
         <v>1231</v>
       </c>
       <c r="D423" s="2" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="E423" s="2" t="s">
         <v>793</v>
@@ -18011,7 +18015,7 @@
         <v>1248</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="E431" s="2"/>
       <c r="F431" s="2"/>
@@ -18177,7 +18181,7 @@
         <v>1267</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="E439" s="2" t="s">
         <v>33</v>
@@ -18775,7 +18779,7 @@
         <v>1358</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="E467" s="2"/>
       <c r="F467" s="2" t="s">
@@ -18865,7 +18869,7 @@
         <v>1374</v>
       </c>
       <c r="D471" s="2" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="E471" s="2" t="s">
         <v>141</v>
@@ -18909,7 +18913,7 @@
         <v>1381</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="E473" s="2" t="s">
         <v>141</v>
@@ -19079,7 +19083,7 @@
         <v>1405</v>
       </c>
       <c r="D481" s="2" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="E481" s="2" t="s">
         <v>1406</v>
@@ -19121,7 +19125,7 @@
         <v>1411</v>
       </c>
       <c r="D483" s="2" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="E483" s="2" t="s">
         <v>1412</v>
@@ -19249,7 +19253,7 @@
         <v>1431</v>
       </c>
       <c r="D489" s="2" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="E489" s="2" t="s">
         <v>75</v>
@@ -19450,7 +19454,7 @@
         <v>1462</v>
       </c>
       <c r="D498" s="2" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="E498" s="2" t="s">
         <v>158</v>
@@ -19494,7 +19498,7 @@
         <v>1469</v>
       </c>
       <c r="D500" s="2" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="E500" s="2" t="s">
         <v>1471</v>
@@ -19603,7 +19607,7 @@
         <v>1488</v>
       </c>
       <c r="D505" s="2" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="E505" s="2" t="s">
         <v>311</v>
@@ -19645,7 +19649,7 @@
         <v>1494</v>
       </c>
       <c r="D507" s="2" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="E507" s="2" t="s">
         <v>468</v>
@@ -19687,7 +19691,7 @@
         <v>1499</v>
       </c>
       <c r="D509" s="2" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="E509" s="2" t="s">
         <v>1500</v>
@@ -19708,7 +19712,7 @@
         <v>1502</v>
       </c>
       <c r="D510" s="2" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="E510" s="2" t="s">
         <v>99</v>
@@ -19796,7 +19800,7 @@
         <v>1513</v>
       </c>
       <c r="D514" s="1" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="E514" s="2" t="s">
         <v>78</v>
@@ -19859,7 +19863,7 @@
         <v>1519</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="E517" s="2" t="s">
         <v>1520</v>
@@ -19901,7 +19905,7 @@
         <v>1526</v>
       </c>
       <c r="D519" s="2" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E519" s="2" t="s">
         <v>141</v>
@@ -20117,7 +20121,7 @@
         <v>1552</v>
       </c>
       <c r="D529" s="2" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="E529" s="2" t="s">
         <v>1553</v>
@@ -20187,7 +20191,7 @@
         <v>367</v>
       </c>
       <c r="E532" s="2" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="F532" s="2"/>
       <c r="G532" s="7" t="s">
@@ -20763,7 +20767,7 @@
         <v>1640</v>
       </c>
       <c r="D559" s="2" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="E559" s="2" t="s">
         <v>208</v>
@@ -20808,7 +20812,7 @@
         <v>2463</v>
       </c>
       <c r="E561" s="2" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="F561" s="2" t="s">
         <v>1648</v>
@@ -20979,7 +20983,7 @@
         <v>1673</v>
       </c>
       <c r="D569" s="2" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="E569" s="2" t="s">
         <v>665</v>
@@ -21088,7 +21092,7 @@
         <v>1686</v>
       </c>
       <c r="D574" s="2" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="E574" s="2" t="s">
         <v>208</v>
@@ -21132,7 +21136,7 @@
         <v>1691</v>
       </c>
       <c r="D576" s="2" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="E576" s="2" t="s">
         <v>58</v>
@@ -21172,7 +21176,7 @@
         <v>1695</v>
       </c>
       <c r="D578" s="2" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="E578" s="2"/>
       <c r="F578" s="2" t="s">
@@ -21238,7 +21242,7 @@
         <v>1704</v>
       </c>
       <c r="E581" s="2" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="F581" s="2" t="s">
         <v>1705</v>
@@ -21390,7 +21394,7 @@
         <v>1724</v>
       </c>
       <c r="D588" s="2" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="E588" s="2" t="s">
         <v>1725</v>
@@ -21413,7 +21417,7 @@
         <v>1728</v>
       </c>
       <c r="D589" s="2" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="E589" s="2" t="s">
         <v>1729</v>
@@ -21434,7 +21438,7 @@
         <v>1731</v>
       </c>
       <c r="D590" s="2" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="E590" s="2" t="s">
         <v>78</v>
@@ -21591,10 +21595,10 @@
         <v>1756</v>
       </c>
       <c r="D597" s="2" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="E597" s="2" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="F597" s="2"/>
       <c r="G597" s="7" t="s">
@@ -21678,7 +21682,7 @@
         <v>1765</v>
       </c>
       <c r="E601" s="2" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="F601" s="2"/>
       <c r="G601" s="7" t="s">
@@ -21740,7 +21744,7 @@
         <v>1774</v>
       </c>
       <c r="D604" s="2" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="E604" s="2" t="s">
         <v>47</v>
@@ -21894,7 +21898,7 @@
         <v>1795</v>
       </c>
       <c r="E611" s="2" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="F611" s="2"/>
       <c r="G611" s="7" t="s">
@@ -21912,7 +21916,7 @@
         <v>1797</v>
       </c>
       <c r="D612" s="2" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="E612" s="2" t="s">
         <v>1798</v>
@@ -22060,7 +22064,7 @@
         <v>1814</v>
       </c>
       <c r="E619" s="2" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="F619" s="2"/>
       <c r="G619" s="7" t="s">
@@ -22246,10 +22250,10 @@
         <v>1840</v>
       </c>
       <c r="D628" s="2" t="s">
+        <v>2553</v>
+      </c>
+      <c r="E628" s="2" t="s">
         <v>2554</v>
-      </c>
-      <c r="E628" s="2" t="s">
-        <v>2555</v>
       </c>
       <c r="F628" s="2" t="s">
         <v>1841</v>
@@ -22606,7 +22610,7 @@
         <v>1886</v>
       </c>
       <c r="E645" s="2" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="F645" s="2"/>
       <c r="G645" s="7" t="s">
@@ -22712,7 +22716,7 @@
         <v>1903</v>
       </c>
       <c r="D650" s="2" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="E650" s="2" t="s">
         <v>1904</v>
@@ -22865,10 +22869,10 @@
         <v>1926</v>
       </c>
       <c r="D657" s="2" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="E657" s="2" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="F657" s="2" t="s">
         <v>1927</v>
@@ -22891,7 +22895,7 @@
         <v>1930</v>
       </c>
       <c r="E658" s="2" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="F658" s="2"/>
       <c r="G658" s="7" t="s">
@@ -22953,7 +22957,7 @@
         <v>1940</v>
       </c>
       <c r="D661" s="2" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="E661" s="2" t="s">
         <v>78</v>
@@ -23039,7 +23043,7 @@
         <v>1952</v>
       </c>
       <c r="D665" s="2" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="E665" s="2" t="s">
         <v>220</v>
@@ -23167,7 +23171,7 @@
         <v>1969</v>
       </c>
       <c r="D671" s="2" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="E671" s="2" t="s">
         <v>1970</v>
@@ -23234,7 +23238,7 @@
         <v>1979</v>
       </c>
       <c r="D674" s="2" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="E674" s="2" t="s">
         <v>208</v>
@@ -23946,7 +23950,7 @@
         <v>2064</v>
       </c>
       <c r="D708" s="2" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="E708" s="2"/>
       <c r="F708" s="2"/>
@@ -24073,7 +24077,7 @@
         <v>2416</v>
       </c>
       <c r="E714" s="2" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="F714" s="2" t="s">
         <v>2081</v>
@@ -24183,7 +24187,7 @@
         <v>2097</v>
       </c>
       <c r="D719" s="2" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="E719" s="2" t="s">
         <v>208</v>
@@ -24204,10 +24208,10 @@
         <v>2100</v>
       </c>
       <c r="D720" s="2" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="E720" s="2" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="F720" s="2" t="s">
         <v>2101</v>
@@ -24253,7 +24257,7 @@
         <v>2108</v>
       </c>
       <c r="E722" s="2" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="F722" s="2" t="s">
         <v>2109</v>
@@ -24294,7 +24298,7 @@
         <v>2114</v>
       </c>
       <c r="D724" s="2" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="E724" s="2" t="s">
         <v>793</v>
@@ -24315,7 +24319,7 @@
         <v>2116</v>
       </c>
       <c r="D725" s="2" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="E725" s="2" t="s">
         <v>47</v>
@@ -24341,7 +24345,7 @@
         <v>2120</v>
       </c>
       <c r="E726" s="2" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="F726" s="2" t="s">
         <v>2121</v>
@@ -24361,7 +24365,7 @@
         <v>2123</v>
       </c>
       <c r="D727" s="2" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="E727" s="2" t="s">
         <v>793</v>
@@ -24385,7 +24389,7 @@
         <v>1463</v>
       </c>
       <c r="E728" s="2" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="F728" s="2" t="s">
         <v>2126</v>
@@ -24496,7 +24500,7 @@
         <v>2420</v>
       </c>
       <c r="E733" s="2" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="F733" s="2" t="s">
         <v>2144</v>
@@ -24516,7 +24520,7 @@
         <v>2146</v>
       </c>
       <c r="D734" s="2" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="E734" s="2" t="s">
         <v>2147</v>
@@ -25049,7 +25053,7 @@
         <v>2209</v>
       </c>
       <c r="D759" s="2" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="E759" s="2" t="s">
         <v>220</v>
@@ -25072,7 +25076,7 @@
         <v>2212</v>
       </c>
       <c r="D760" s="2" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="E760" s="2" t="s">
         <v>2213</v>
@@ -25117,7 +25121,7 @@
         <v>815</v>
       </c>
       <c r="E762" s="2" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="F762" s="2"/>
       <c r="G762" s="7" t="s">
@@ -26174,7 +26178,7 @@
     </row>
     <row r="815" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A815" s="2" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="B815" s="2" t="s">
         <v>8</v>
@@ -26195,7 +26199,7 @@
     </row>
     <row r="816" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A816" s="2" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="B816" s="2" t="s">
         <v>446</v>
@@ -26216,7 +26220,7 @@
     </row>
     <row r="817" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A817" s="2" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="B817" s="2" t="s">
         <v>8</v>
@@ -26237,7 +26241,7 @@
     </row>
     <row r="818" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A818" s="2" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="B818" s="2" t="s">
         <v>532</v>
@@ -26258,7 +26262,7 @@
     </row>
     <row r="819" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A819" s="2" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="B819" s="2" t="s">
         <v>532</v>
@@ -26279,7 +26283,7 @@
     </row>
     <row r="820" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A820" s="2" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="B820" s="2" t="s">
         <v>8</v>
@@ -26300,7 +26304,7 @@
     </row>
     <row r="821" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A821" s="2" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="B821" s="2" t="s">
         <v>14</v>
@@ -26319,7 +26323,7 @@
     </row>
     <row r="822" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A822" s="2" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="B822" s="2" t="s">
         <v>14</v>
@@ -26338,7 +26342,7 @@
     </row>
     <row r="823" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A823" s="2" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="B823" s="2" t="s">
         <v>8</v>
@@ -26359,7 +26363,7 @@
     </row>
     <row r="824" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A824" s="2" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="B824" s="2" t="s">
         <v>14</v>
@@ -26382,7 +26386,7 @@
     </row>
     <row r="825" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A825" s="2" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>8</v>
@@ -26401,7 +26405,7 @@
     </row>
     <row r="826" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A826" s="2" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="B826" s="2" t="s">
         <v>8</v>
@@ -26420,7 +26424,7 @@
     </row>
     <row r="827" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A827" s="2" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="B827" s="2" t="s">
         <v>8</v>
@@ -26441,7 +26445,7 @@
     </row>
     <row r="828" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A828" s="2" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="B828" s="2" t="s">
         <v>14</v>
@@ -26464,7 +26468,7 @@
     </row>
     <row r="829" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A829" s="2" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="B829" s="2" t="s">
         <v>8</v>
@@ -26483,7 +26487,7 @@
     </row>
     <row r="830" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A830" s="2" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="B830" s="2" t="s">
         <v>14</v>
@@ -26504,7 +26508,7 @@
     </row>
     <row r="831" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A831" s="2" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="B831" s="2" t="s">
         <v>446</v>
@@ -26527,7 +26531,7 @@
     </row>
     <row r="832" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A832" s="2" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="B832" s="2" t="s">
         <v>446</v>
@@ -26550,7 +26554,7 @@
     </row>
     <row r="833" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A833" s="2" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="B833" s="2" t="s">
         <v>8</v>
@@ -26571,7 +26575,7 @@
     </row>
     <row r="834" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A834" s="2" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="B834" s="2" t="s">
         <v>446</v>
@@ -26590,7 +26594,7 @@
     </row>
     <row r="835" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A835" s="2" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="B835" s="2" t="s">
         <v>446</v>
@@ -26609,7 +26613,7 @@
     </row>
     <row r="836" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A836" s="2" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="B836" s="2" t="s">
         <v>14</v>
@@ -26628,7 +26632,7 @@
     </row>
     <row r="837" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A837" s="2" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="B837" s="2" t="s">
         <v>446</v>
@@ -26647,7 +26651,7 @@
     </row>
     <row r="838" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A838" s="2" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="B838" s="2" t="s">
         <v>14</v>
@@ -26666,7 +26670,7 @@
     </row>
     <row r="839" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A839" s="2" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="B839" s="2" t="s">
         <v>446</v>
@@ -26689,7 +26693,7 @@
     </row>
     <row r="840" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A840" s="2" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="B840" s="2" t="s">
         <v>709</v>
@@ -26708,7 +26712,7 @@
     </row>
     <row r="841" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A841" s="2" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="B841" s="2" t="s">
         <v>446</v>
@@ -26729,7 +26733,7 @@
     </row>
     <row r="842" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A842" s="2" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="B842" s="2" t="s">
         <v>14</v>
@@ -26752,7 +26756,7 @@
     </row>
     <row r="843" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A843" s="2" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="B843" s="2" t="s">
         <v>14</v>
@@ -26771,7 +26775,7 @@
     </row>
     <row r="844" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A844" s="2" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="B844" s="2" t="s">
         <v>14</v>
@@ -26792,7 +26796,7 @@
     </row>
     <row r="845" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A845" s="2" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="B845" s="2" t="s">
         <v>971</v>
@@ -26811,7 +26815,7 @@
     </row>
     <row r="846" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A846" s="2" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="B846" s="2" t="s">
         <v>14</v>
@@ -26832,7 +26836,7 @@
     </row>
     <row r="847" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A847" s="2" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="B847" s="2" t="s">
         <v>14</v>
@@ -26855,7 +26859,7 @@
     </row>
     <row r="848" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A848" s="2" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B848" s="2" t="s">
         <v>8</v>
@@ -26876,7 +26880,7 @@
     </row>
     <row r="849" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A849" s="2" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="B849" s="2" t="s">
         <v>14</v>
@@ -26897,7 +26901,7 @@
     </row>
     <row r="850" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A850" s="2" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="B850" s="2" t="s">
         <v>8</v>
@@ -26916,7 +26920,7 @@
     </row>
     <row r="851" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A851" s="2" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="B851" s="2" t="s">
         <v>446</v>
@@ -26937,7 +26941,7 @@
     </row>
     <row r="852" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A852" s="2" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="B852" s="2" t="s">
         <v>496</v>
@@ -26958,7 +26962,7 @@
     </row>
     <row r="853" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A853" s="2" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="B853" s="2" t="s">
         <v>446</v>
@@ -26970,16 +26974,16 @@
         <v>2416</v>
       </c>
       <c r="E853" s="2" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="F853" s="2"/>
       <c r="G853" s="7" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="854" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A854" s="2" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="B854" s="3" t="s">
         <v>496</v>
@@ -26988,7 +26992,7 @@
         <v>2386</v>
       </c>
       <c r="D854" s="3" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="E854" s="8"/>
       <c r="F854" s="9" t="s">
@@ -27000,7 +27004,7 @@
     </row>
     <row r="855" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A855" s="2" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="B855" s="3" t="s">
         <v>496</v>
@@ -27023,7 +27027,7 @@
     </row>
     <row r="856" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A856" s="2" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="B856" s="3" t="s">
         <v>571</v>
@@ -27035,7 +27039,7 @@
         <v>2391</v>
       </c>
       <c r="E856" s="11" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="F856" s="8"/>
       <c r="G856" s="7" t="s">
@@ -27044,7 +27048,7 @@
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A857" s="2" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="B857" s="3" t="s">
         <v>571</v>
@@ -27067,7 +27071,7 @@
     </row>
     <row r="858" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A858" s="2" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="B858" s="3" t="s">
         <v>496</v>
@@ -27088,7 +27092,7 @@
     </row>
     <row r="859" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A859" s="2" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="B859" s="3" t="s">
         <v>496</v>
@@ -27107,7 +27111,7 @@
     </row>
     <row r="860" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A860" s="2" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="B860" s="3" t="s">
         <v>496</v>
@@ -27128,7 +27132,7 @@
     </row>
     <row r="861" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A861" s="2" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="B861" s="3" t="s">
         <v>557</v>
@@ -27149,7 +27153,7 @@
     </row>
     <row r="862" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A862" s="2" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="B862" s="3" t="s">
         <v>496</v>
@@ -27158,7 +27162,7 @@
         <v>2398</v>
       </c>
       <c r="D862" s="3" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="E862" s="8"/>
       <c r="F862" s="8"/>
@@ -27168,7 +27172,7 @@
     </row>
     <row r="863" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A863" s="2" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="B863" s="3" t="s">
         <v>557</v>
@@ -27189,7 +27193,7 @@
     </row>
     <row r="864" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A864" s="2" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="B864" s="3" t="s">
         <v>998</v>
@@ -27210,7 +27214,7 @@
     </row>
     <row r="865" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A865" s="2" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="B865" s="3" t="s">
         <v>971</v>
@@ -27231,7 +27235,7 @@
     </row>
     <row r="866" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A866" s="2" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="B866" s="3" t="s">
         <v>14</v>
@@ -27243,7 +27247,7 @@
         <v>815</v>
       </c>
       <c r="E866" s="11" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="F866" s="8"/>
       <c r="G866" s="7" t="s">
@@ -27252,7 +27256,7 @@
     </row>
     <row r="867" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A867" s="2" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="B867" s="3" t="s">
         <v>14</v>
@@ -27264,7 +27268,7 @@
         <v>359</v>
       </c>
       <c r="E867" s="11" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="F867" s="11" t="s">
         <v>2405</v>

</xml_diff>

<commit_message>
20160407 bug fix and unit fix
</commit_message>
<xml_diff>
--- a/res/east20160309.xlsx
+++ b/res/east20160309.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5306" uniqueCount="2625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5308" uniqueCount="2626">
   <si>
     <t/>
   </si>
@@ -8419,6 +8419,10 @@
   </si>
   <si>
     <t>条,公斤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8846,8 +8850,8 @@
   <dimension ref="A1:G994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G260" sqref="G260"/>
+      <pane ySplit="1" topLeftCell="A848" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G790" sqref="G790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -26081,7 +26085,9 @@
       </c>
       <c r="E809" s="2"/>
       <c r="F809" s="2"/>
-      <c r="G809" s="7"/>
+      <c r="G809" s="7" t="s">
+        <v>2625</v>
+      </c>
     </row>
     <row r="810" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A810" s="2" t="s">
@@ -26098,7 +26104,9 @@
       </c>
       <c r="E810" s="2"/>
       <c r="F810" s="2"/>
-      <c r="G810" s="7"/>
+      <c r="G810" s="7" t="s">
+        <v>2625</v>
+      </c>
     </row>
     <row r="811" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A811" s="2" t="s">

</xml_diff>